<commit_message>
Add data to sheets
Add missing values of model name and reference quaternions
</commit_message>
<xml_diff>
--- a/iRT gsheets.xlsx
+++ b/iRT gsheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Documents\GitHub\octave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D524BFE-3B0B-4DB6-9ABA-7B7408B6050E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB963D7-059B-4844-B3F0-B3DD917F4995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3810" yWindow="2640" windowWidth="14055" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -48,6 +48,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Data do recebimento dos dados pela planilha
@@ -62,6 +63,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Email da pessoa
@@ -76,6 +78,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Nome da pessoa
@@ -90,6 +93,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Identificador da tarefa realizada.
@@ -104,6 +108,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Razão entre pixels da tela e unidades de distância entre os vértices (no Jmol é em Angstroms)
@@ -118,6 +123,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Unix Epoch partindo do início de cada tarefa.
@@ -133,6 +139,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Duração da tarefa
@@ -147,6 +154,7 @@
             <sz val="10"/>
             <color rgb="FF000000"/>
             <rFont val="Calibri"/>
+            <family val="2"/>
             <scheme val="minor"/>
           </rPr>
           <t>Coordenadas de orientação em quatérnio (a + bi + cj + dk).
@@ -160,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
   <si>
     <t>timestamp</t>
   </si>
@@ -364,6 +372,27 @@
   </si>
   <si>
     <t>1,1,1,1,1,1,1,1,1,1,1,1,1,0.99303,0.989593,0.98547,0.979636,0.977837,0.972432,0.972027,0.969928,0.969928,0.969928,0.985713,0.99027,0.99395,0.998514,0.999353,0.994517,0.986225,0.981817,0.977878,0.976649,0.979189,0.990351,0.983287,0.974495,0.960717,0.951575,0.918227,0.900512,0.897022,0.891175,0.886912,0.882597,0.864363,0.844796,0.815782,0.804849,0.798486,0.798486,0.798486,0.798486,0.798486,0.861553,0.909397,0.944731,0.958142,0.965658,0.965464,0.960079,0.933446,0.922116,0.90307,0.893065,0.878979,0.87238,0.86757,0.873807,0.876168,0.876168,0.876168,0.876168,0.876168,0.876168,0.858753,0.846672,0.845812,0.849321,0.852613,0.869176,0.872969,0.884915,0.907965,0.920284,0.925413,0.930279,0.939321,0.943495,0.949101,0.950788,0.949803,0.942554,0.926532,0.915972,0.909998,0.907431,0.907693,0.899722,0.891339,0.881186,0.87591,0.873283,0.873283,0.873283,0.873283,0.873283,0.880993,0.884783,0.885482,0.886327,0.895041,0.906624,0.925428,0.929724,0.930762,0.932359,0.932444,0.929004,0.928035,0.924691,0.921242,0.91986,0.91986,0.917545,0.915174,0.915174,0.915174,0.915174,0.912383,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.911132,0.919401,0.919401,0.919401,0.919401,0.919401,0.919401,0.919401,0.919401,0.919401,0.919401,0.919401,0.919401,0.919401,0.919401,0.919401,0.915777,0.915777,0.914955,0.914955,0.914955,0.912403,0.912403,0.912403,0.911524,0.911524,0.911524,0.911524,0.911524,0.911524,0.912403,0.914503,0.920486,0.920486,0.923618,0.925566,0.925566,0.925566,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.921755,0.923335,0.924104,0.927504,0.927504,0.929386,0.935043,0.935043,0.935043,0.935043,0.933633,0.924174,0.922979,0.922979,0.922979,0.922979,0.922979,0.922979,0.922979,0.922979,0.922979,0.922979,0.922979,0.922979,0.918057,0.918057,0.918057,0.918057,0.918057,0.918057,0.918057,0.918057,0.920547,0.920995,0.920995,0.920995,0.920995,0.920995,0.920995,0.920995,0.920995,0.920995,0.920995,0.920995,0.920995,0.920995,0.920207,0.920207,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.91859,0.920995,0.922527,0.922527,0.923272,0.923272,0.920537,0.918972,0.915673,0.915673,0.915673,0.915673,0.914813,0.914813,0.914813,0.914813,0.914813,0.914813,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.913939,0.911483,0.907693,0.906401,0.90771,0.911803,0.916147,0.920877,0.923444,0.927732,0.928732,0.921438,0.914431,0.908937,0.904748,0.903449,0.904321,0.905179,0.910035,0.912159,0.916166,0.920561,0.921049,0.918276,0.913303,0.910218,0.902599,0.896761,0.890509,0.8941,0.899865,0.902561,0.905662,0.913168,0.915737,0.917422,0.91486,0.906181,0.898358,0.892583,0.888655,0.893379,0.897312,0.902847,0.911242,0.912523,0.916282,0.915408,0.915408,0.915408,0.915408,0.920215,0.920215,0.920215,0.920215,0.920215,0.920215,0.919903,0.919903,0.919903,0.919903,0.919903,0.919903,0.921085,0.92426,0.92426,0.92426,0.92426,0.921934,0.921934,0.921934,0.921934,0.921934,0.921934,0.921934,0.921934,0.921934,0.921934,0.921082,0.921082,0.921082,0.921082,0.921082,0.921082,0.921082,0.921082,0.921082,0.921082,0.92225,0.923404,0.923404,0.923404,0.923404,0.923404,0.923404,0.92225,0.92225,0.913637,0.913637,0.913637,0.914857,0.914857,0.916962,0.916962,0.916962,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.917847,0.919042,0.920222,0.918446,0.918446,0.918446,0.918446,0.918446,0.918446,0.920505,0.920505,0.920505,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.922535,0.919036,0.919036,0.919036,0.917841,0.917841,0.912921,0.912921,0.912921,0.912921,0.91541,0.917841,0.917841,0.917841,0.917841,0.919906,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943,0.921943</t>
+  </si>
+  <si>
+    <t>modelName</t>
+  </si>
+  <si>
+    <t>pseudobatracotoxin_molecule.xyz</t>
+  </si>
+  <si>
+    <t>MRT_VK_mol.xyz</t>
+  </si>
+  <si>
+    <t>ref_i</t>
+  </si>
+  <si>
+    <t>ref_j</t>
+  </si>
+  <si>
+    <t>ref_k</t>
+  </si>
+  <si>
+    <t>ref_r</t>
   </si>
 </sst>
 </file>
@@ -385,17 +414,20 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Consolas"/>
+      <family val="3"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -708,7 +740,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,11 +785,21 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="2"/>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2"/>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2"/>
+      <c r="N1" t="s">
+        <v>71</v>
+      </c>
+      <c r="O1" t="s">
+        <v>72</v>
+      </c>
+      <c r="P1" t="s">
+        <v>73</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>74</v>
+      </c>
+      <c r="R1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3">
@@ -797,11 +839,21 @@
       <c r="M2" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="N2" s="2"/>
-      <c r="O2" s="2"/>
-      <c r="P2" s="2"/>
-      <c r="Q2" s="2"/>
-      <c r="R2" s="2"/>
+      <c r="N2">
+        <v>-0.490257597533579</v>
+      </c>
+      <c r="O2">
+        <v>-0.28253363768972101</v>
+      </c>
+      <c r="P2">
+        <v>-0.45539483504230199</v>
+      </c>
+      <c r="Q2">
+        <v>0.68734109134490795</v>
+      </c>
+      <c r="R2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="3">
@@ -841,11 +893,21 @@
       <c r="M3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="N3" s="2"/>
-      <c r="O3" s="2"/>
-      <c r="P3" s="2"/>
-      <c r="Q3" s="2"/>
-      <c r="R3" s="2"/>
+      <c r="N3">
+        <v>-0.490257597533579</v>
+      </c>
+      <c r="O3">
+        <v>-0.28253363768972101</v>
+      </c>
+      <c r="P3">
+        <v>-0.45539483504230199</v>
+      </c>
+      <c r="Q3">
+        <v>0.68734109134490795</v>
+      </c>
+      <c r="R3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="3">
@@ -885,11 +947,21 @@
       <c r="M4" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="N4" s="2"/>
-      <c r="O4" s="2"/>
-      <c r="P4" s="2"/>
-      <c r="Q4" s="2"/>
-      <c r="R4" s="2"/>
+      <c r="N4">
+        <v>0.29922234471855402</v>
+      </c>
+      <c r="O4">
+        <v>0.223654136694591</v>
+      </c>
+      <c r="P4">
+        <v>-0.10297736856098801</v>
+      </c>
+      <c r="Q4">
+        <v>0.92186792824394204</v>
+      </c>
+      <c r="R4" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="3">
@@ -929,11 +1001,21 @@
       <c r="M5" s="4" t="s">
         <v>51</v>
       </c>
-      <c r="N5" s="2"/>
-      <c r="O5" s="2"/>
-      <c r="P5" s="2"/>
-      <c r="Q5" s="2"/>
-      <c r="R5" s="2"/>
+      <c r="N5">
+        <v>-0.490257597533579</v>
+      </c>
+      <c r="O5">
+        <v>-0.28253363768972101</v>
+      </c>
+      <c r="P5">
+        <v>-0.45539483504230199</v>
+      </c>
+      <c r="Q5">
+        <v>0.68734109134490795</v>
+      </c>
+      <c r="R5" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="3">
@@ -973,11 +1055,21 @@
       <c r="M6" s="4" t="s">
         <v>59</v>
       </c>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
+      <c r="N6">
+        <v>-0.490257597533579</v>
+      </c>
+      <c r="O6">
+        <v>-0.28253363768972101</v>
+      </c>
+      <c r="P6">
+        <v>-0.45539483504230199</v>
+      </c>
+      <c r="Q6">
+        <v>0.68734109134490795</v>
+      </c>
+      <c r="R6" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="3">
@@ -1017,11 +1109,21 @@
       <c r="M7" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
+      <c r="N7">
+        <v>0.29922234471855402</v>
+      </c>
+      <c r="O7">
+        <v>0.223654136694591</v>
+      </c>
+      <c r="P7">
+        <v>-0.10297736856098801</v>
+      </c>
+      <c r="Q7">
+        <v>0.92186792824394204</v>
+      </c>
+      <c r="R7" t="s">
+        <v>70</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Months of progress and a data fix to iRT gsheets.xlsx
Months of progress and a data fix (one value of pxAngstRatio was wrong)
</commit_message>
<xml_diff>
--- a/iRT gsheets.xlsx
+++ b/iRT gsheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rodrigo\Documents\GitHub\octave\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CB963D7-059B-4844-B3F0-B3DD917F4995}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EED0D49-9B96-48D4-A8AA-8B8F71FF5152}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3810" yWindow="2640" windowWidth="14055" windowHeight="12555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="74">
   <si>
     <t>timestamp</t>
   </si>
@@ -243,9 +243,6 @@
   </si>
   <si>
     <t>poligonFill</t>
-  </si>
-  <si>
-    <t>13.092058078903449,-19.751618968223273</t>
   </si>
   <si>
     <t>1682705349098</t>
@@ -740,7 +737,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,19 +783,19 @@
         <v>12</v>
       </c>
       <c r="N1" t="s">
+        <v>70</v>
+      </c>
+      <c r="O1" t="s">
         <v>71</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>72</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>73</v>
       </c>
-      <c r="Q1" t="s">
-        <v>74</v>
-      </c>
       <c r="R1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
@@ -852,7 +849,7 @@
         <v>0.68734109134490795</v>
       </c>
       <c r="R2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.25">
@@ -870,28 +867,28 @@
         <v>24</v>
       </c>
       <c r="F3" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="G3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="4" t="s">
+      <c r="J3" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>29</v>
       </c>
-      <c r="K3" s="4" t="s">
+      <c r="L3" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L3" s="4" t="s">
+      <c r="M3" s="4" t="s">
         <v>31</v>
-      </c>
-      <c r="M3" s="4" t="s">
-        <v>32</v>
       </c>
       <c r="N3">
         <v>-0.490257597533579</v>
@@ -906,7 +903,7 @@
         <v>0.68734109134490795</v>
       </c>
       <c r="R3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
@@ -921,31 +918,31 @@
         <v>14</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="4" t="s">
+      <c r="H4" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="H4" s="4" t="s">
+      <c r="I4" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="4" t="s">
+      <c r="J4" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K4" s="4" t="s">
+      <c r="L4" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="4" t="s">
+      <c r="M4" s="4" t="s">
         <v>40</v>
-      </c>
-      <c r="M4" s="4" t="s">
-        <v>41</v>
       </c>
       <c r="N4">
         <v>0.29922234471855402</v>
@@ -960,7 +957,7 @@
         <v>0.92186792824394204</v>
       </c>
       <c r="R4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -969,37 +966,37 @@
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
       <c r="F5" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="H5" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="H5" s="4" t="s">
+      <c r="I5" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="I5" s="4" t="s">
+      <c r="J5" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="4" t="s">
+      <c r="K5" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="K5" s="4" t="s">
+      <c r="L5" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="L5" s="4" t="s">
+      <c r="M5" s="4" t="s">
         <v>50</v>
-      </c>
-      <c r="M5" s="4" t="s">
-        <v>51</v>
       </c>
       <c r="N5">
         <v>-0.490257597533579</v>
@@ -1014,7 +1011,7 @@
         <v>0.68734109134490795</v>
       </c>
       <c r="R5" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -1023,37 +1020,37 @@
       </c>
       <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>42</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>43</v>
       </c>
       <c r="E6" s="4" t="s">
         <v>24</v>
       </c>
       <c r="F6" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="G6" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="H6" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="H6" s="4" t="s">
+      <c r="I6" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="I6" s="4" t="s">
+      <c r="J6" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="J6" s="4" t="s">
+      <c r="K6" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="K6" s="4" t="s">
+      <c r="L6" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="L6" s="4" t="s">
+      <c r="M6" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="M6" s="4" t="s">
-        <v>59</v>
       </c>
       <c r="N6">
         <v>-0.490257597533579</v>
@@ -1068,7 +1065,7 @@
         <v>0.68734109134490795</v>
       </c>
       <c r="R6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -1077,37 +1074,37 @@
       </c>
       <c r="B7" s="4"/>
       <c r="C7" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="4" t="s">
-        <v>43</v>
-      </c>
       <c r="E7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F7" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="G7" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="H7" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="H7" s="4" t="s">
+      <c r="I7" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I7" s="4" t="s">
+      <c r="J7" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="J7" s="4" t="s">
+      <c r="K7" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="K7" s="4" t="s">
+      <c r="L7" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="L7" s="4" t="s">
+      <c r="M7" s="4" t="s">
         <v>66</v>
-      </c>
-      <c r="M7" s="4" t="s">
-        <v>67</v>
       </c>
       <c r="N7">
         <v>0.29922234471855402</v>
@@ -1122,11 +1119,12 @@
         <v>0.92186792824394204</v>
       </c>
       <c r="R7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>